<commit_message>
Documented State Engine and cleaned up internal functionality of State Engine. Moved sdl init flags into SDLUtilityTool and put them inside the sdl utility tool instead of being passed in by the state engine.
</commit_message>
<xml_diff>
--- a/GameSource/GameAgenda.xlsx
+++ b/GameSource/GameAgenda.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>LARGE</t>
   </si>
@@ -35,9 +35,6 @@
     <t>SMALL</t>
   </si>
   <si>
-    <t>Document StateEngine</t>
-  </si>
-  <si>
     <t>Document TileMap</t>
   </si>
   <si>
@@ -45,6 +42,12 @@
   </si>
   <si>
     <t>Determine Texture Sizes</t>
+  </si>
+  <si>
+    <t>Document SDLUtilityTool</t>
+  </si>
+  <si>
+    <t>Document the TileMap, b2world, axis orientations</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +394,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -399,13 +405,14 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished documenting TIleMap and changed minimum tile world size
</commit_message>
<xml_diff>
--- a/GameSource/GameAgenda.xlsx
+++ b/GameSource/GameAgenda.xlsx
@@ -35,19 +35,19 @@
     <t>SMALL</t>
   </si>
   <si>
-    <t>Document TileMap</t>
-  </si>
-  <si>
     <t>Integrate Flyweight model for entities</t>
   </si>
   <si>
-    <t>Determine Texture Sizes</t>
-  </si>
-  <si>
     <t>Document SDLUtilityTool</t>
   </si>
   <si>
     <t>Document the TileMap, b2world, axis orientations</t>
+  </si>
+  <si>
+    <t>Figure out level file format</t>
+  </si>
+  <si>
+    <t>*Determine Texture Sizes</t>
   </si>
 </sst>
 </file>
@@ -368,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,20 +394,22 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added dependency on tinyxml2 for xml parsing, Fixed bug with sdlUtilityTool resource counting (known memory leak in game play state from manual entity creation). Static and Dynamic entity structure partially done.
</commit_message>
<xml_diff>
--- a/GameSource/GameAgenda.xlsx
+++ b/GameSource/GameAgenda.xlsx
@@ -54,10 +54,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,11 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,7 +379,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +401,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">

</xml_diff>

<commit_message>
Many changes to targeting. New data structure that handles targeting, hashtable/linked list hybrid. Entities now fight each other. Next step is multiple fixture entities.
</commit_message>
<xml_diff>
--- a/GameSource/GameAgenda.xlsx
+++ b/GameSource/GameAgenda.xlsx
@@ -35,12 +35,6 @@
     <t>SMALL</t>
   </si>
   <si>
-    <t>Integrate Flyweight model for entities</t>
-  </si>
-  <si>
-    <t>Document SDLUtilityTool</t>
-  </si>
-  <si>
     <t>Document the TileMap, b2world, axis orientations</t>
   </si>
   <si>
@@ -48,6 +42,12 @@
   </si>
   <si>
     <t>*Determine Texture Sizes</t>
+  </si>
+  <si>
+    <t>Research box 2d shapes</t>
+  </si>
+  <si>
+    <t>Figure out format for entities that have only one texture</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,24 +401,25 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>